<commit_message>
Widthdrawl Test case updation
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\eclipse-workspace\DataDrivenFrameWork\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3158F1E-784B-49B5-B69F-6D8605C00AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96B75B4-738E-44A5-B2B5-285AA633D886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
   </bookViews>
   <sheets>
     <sheet name="AddNewCustomerTest" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="successfulCustomerLoginTest" sheetId="6" r:id="rId6"/>
     <sheet name="addDepositTest" sheetId="7" r:id="rId7"/>
     <sheet name="depositVisibleInTransTest" sheetId="8" r:id="rId8"/>
-    <sheet name="test_suite" sheetId="9" r:id="rId9"/>
+    <sheet name="withdrawlAmtLessThanBalTest" sheetId="10" r:id="rId9"/>
+    <sheet name="test_suite" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>firstname</t>
   </si>
@@ -135,6 +136,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>withdrawlAmount</t>
+  </si>
+  <si>
+    <t>withdrawlAmtLessThanBalTest</t>
   </si>
 </sst>
 </file>
@@ -598,6 +605,121 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED3A46F-23AC-4574-80A5-74A49ABFBA95}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FAC235-18DB-4D3A-B918-4C7C6CAADB5C}">
   <dimension ref="A1:B2"/>
@@ -760,7 +882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C2DE09-F846-45FF-8735-1FC6B4BB1680}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -819,108 +941,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED3A46F-23AC-4574-80A5-74A49ABFBA95}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905423A8-DFD2-4463-911A-7A857E1170BC}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>567</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding new scenarios in withdrawl test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\eclipse-workspace\DataDrivenFrameWork\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96B75B4-738E-44A5-B2B5-285AA633D886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2734CAFE-BEBE-48E6-A61E-0B6730BCBBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="9" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
   </bookViews>
   <sheets>
     <sheet name="AddNewCustomerTest" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="addDepositTest" sheetId="7" r:id="rId7"/>
     <sheet name="depositVisibleInTransTest" sheetId="8" r:id="rId8"/>
     <sheet name="withdrawlAmtLessThanBalTest" sheetId="10" r:id="rId9"/>
-    <sheet name="test_suite" sheetId="9" r:id="rId10"/>
+    <sheet name="withdrawlAmtMoreThanBalTest" sheetId="11" r:id="rId10"/>
+    <sheet name="test_suite" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>firstname</t>
   </si>
@@ -142,6 +143,12 @@
   </si>
   <si>
     <t>withdrawlAmtLessThanBalTest</t>
+  </si>
+  <si>
+    <t>errorMsg</t>
+  </si>
+  <si>
+    <t>Transaction Failed. You can not withdraw amount more than the balance.</t>
   </si>
 </sst>
 </file>
@@ -606,10 +613,45 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912BDD8A-0113-4050-840E-8345A2AD3536}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1067</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED3A46F-23AC-4574-80A5-74A49ABFBA95}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -945,7 +987,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding Account Exist Test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\eclipse-workspace\DataDrivenFrameWork\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2734CAFE-BEBE-48E6-A61E-0B6730BCBBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D451C8-61BB-477D-9082-0442E48A8072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="9" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
   </bookViews>
   <sheets>
     <sheet name="AddNewCustomerTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="depositVisibleInTransTest" sheetId="8" r:id="rId8"/>
     <sheet name="withdrawlAmtLessThanBalTest" sheetId="10" r:id="rId9"/>
     <sheet name="withdrawlAmtMoreThanBalTest" sheetId="11" r:id="rId10"/>
-    <sheet name="test_suite" sheetId="9" r:id="rId11"/>
+    <sheet name="AccountExistTest" sheetId="12" r:id="rId11"/>
+    <sheet name="test_suite" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>firstname</t>
   </si>
@@ -136,9 +137,6 @@
     <t>depositVisibleInTransTest</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>withdrawlAmount</t>
   </si>
   <si>
@@ -149,6 +147,24 @@
   </si>
   <si>
     <t>Transaction Failed. You can not withdraw amount more than the balance.</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>noAccountText</t>
+  </si>
+  <si>
+    <t>Rounak Agarwal</t>
+  </si>
+  <si>
+    <t>Please open an account with us.</t>
+  </si>
+  <si>
+    <t>Sapnish Singh</t>
+  </si>
+  <si>
+    <t>Kuntal Chakraborty</t>
   </si>
 </sst>
 </file>
@@ -510,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE9B237-D341-4C61-991C-11C192AD8C56}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912BDD8A-0113-4050-840E-8345A2AD3536}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -628,10 +644,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -639,15 +655,63 @@
         <v>1067</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C357886-E283-4768-8C99-9889B32A4483}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>37</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED3A46F-23AC-4574-80A5-74A49ABFBA95}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -750,7 +814,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -994,7 +1058,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding MultiAccount Id generator test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\eclipse-workspace\DataDrivenFrameWork\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D451C8-61BB-477D-9082-0442E48A8072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1753590-FC3F-4751-9FF8-FAA3A293B71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="12" xr2:uid="{3C899C3D-DF40-4512-A533-FAE22540B899}"/>
   </bookViews>
   <sheets>
     <sheet name="AddNewCustomerTest" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <sheet name="withdrawlAmtLessThanBalTest" sheetId="10" r:id="rId9"/>
     <sheet name="withdrawlAmtMoreThanBalTest" sheetId="11" r:id="rId10"/>
     <sheet name="AccountExistTest" sheetId="12" r:id="rId11"/>
-    <sheet name="test_suite" sheetId="9" r:id="rId12"/>
+    <sheet name="creatingMultiAcctTest" sheetId="13" r:id="rId12"/>
+    <sheet name="correctMultiAccIdGenTest" sheetId="14" r:id="rId13"/>
+    <sheet name="test_suite" sheetId="9" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>firstname</t>
   </si>
@@ -165,6 +167,18 @@
   </si>
   <si>
     <t>Kuntal Chakraborty</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
@@ -526,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE9B237-D341-4C61-991C-11C192AD8C56}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +549,7 @@
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,6 +726,84 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81554353-0402-4256-9754-7405C72C7E86}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA571AAA-C53C-4DA4-8A33-38AFF4C69761}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED3A46F-23AC-4574-80A5-74A49ABFBA95}">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>